<commit_message>
Ploting data with respect to the period chosen
Corrected ploting info but not the most optimized way. Many other mistakes were solved and comments were added to the code with suggestions of future optimization fixes.
</commit_message>
<xml_diff>
--- a/data/Mice_table.xlsx
+++ b/data/Mice_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\GitHub\Mice_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18FE507-AAA7-4193-A1B0-4F42E20CC324}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB9D647-F8B1-495E-92C4-453E120DEAEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D38C1D22-3EA8-4F40-A472-ED4C86E2FE4E}"/>
   </bookViews>
@@ -57,127 +57,127 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Mouse_1033</t>
+  </si>
+  <si>
+    <t>NP</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Heterozygous</t>
+  </si>
+  <si>
+    <t>Alive</t>
+  </si>
+  <si>
+    <t>Mouse_1032</t>
+  </si>
+  <si>
+    <t>Mouse_OG_WT1</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Wildtype</t>
+  </si>
+  <si>
+    <t>Mouse_OG_WT2</t>
+  </si>
+  <si>
+    <t>LP</t>
+  </si>
+  <si>
+    <t>Mouse_OG_WT3</t>
+  </si>
+  <si>
+    <t>RP</t>
+  </si>
+  <si>
+    <t>Mouse_OG_WT4</t>
+  </si>
+  <si>
+    <t>RLP</t>
+  </si>
+  <si>
+    <t>Mouse_OG_WT5</t>
+  </si>
+  <si>
+    <t>Mouse_OG_WT6</t>
+  </si>
+  <si>
+    <t>Mouse_G1</t>
+  </si>
+  <si>
+    <t>Mouse_G2</t>
+  </si>
+  <si>
+    <t>Mouse_G3</t>
+  </si>
+  <si>
+    <t>Mouse_G4</t>
+  </si>
+  <si>
+    <t>Mouse_G5</t>
+  </si>
+  <si>
+    <t>Mouse_G6</t>
+  </si>
+  <si>
+    <t>Mouse_G7</t>
+  </si>
+  <si>
+    <t>Mouse_G8</t>
+  </si>
+  <si>
+    <t>Mouse_G9</t>
+  </si>
+  <si>
+    <t>Mouse_G10</t>
+  </si>
+  <si>
+    <t>Mouse_G11</t>
+  </si>
+  <si>
+    <t>Mouse_G12</t>
+  </si>
+  <si>
+    <t>RRP</t>
+  </si>
+  <si>
+    <t>Mouse_G13</t>
+  </si>
+  <si>
+    <t>LLP</t>
+  </si>
+  <si>
+    <t>Mouse_G14</t>
+  </si>
+  <si>
+    <t>RRLP</t>
+  </si>
+  <si>
+    <t>Mouse_G15</t>
+  </si>
+  <si>
+    <t>Mouse_G16</t>
+  </si>
+  <si>
+    <t>Mouse_G17</t>
+  </si>
+  <si>
+    <t>Mouse_G18</t>
+  </si>
+  <si>
+    <t>Mouse_G19</t>
+  </si>
+  <si>
+    <t>Mouse_G20</t>
+  </si>
+  <si>
     <t>Age_(days)</t>
-  </si>
-  <si>
-    <t>Mouse_1033</t>
-  </si>
-  <si>
-    <t>NP</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Heterozygous</t>
-  </si>
-  <si>
-    <t>Alive</t>
-  </si>
-  <si>
-    <t>Mouse_1032</t>
-  </si>
-  <si>
-    <t>Mouse_OG_WT1</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>Wildtype</t>
-  </si>
-  <si>
-    <t>Mouse_OG_WT2</t>
-  </si>
-  <si>
-    <t>LP</t>
-  </si>
-  <si>
-    <t>Mouse_OG_WT3</t>
-  </si>
-  <si>
-    <t>RP</t>
-  </si>
-  <si>
-    <t>Mouse_OG_WT4</t>
-  </si>
-  <si>
-    <t>RLP</t>
-  </si>
-  <si>
-    <t>Mouse_OG_WT5</t>
-  </si>
-  <si>
-    <t>Mouse_OG_WT6</t>
-  </si>
-  <si>
-    <t>Mouse_G1</t>
-  </si>
-  <si>
-    <t>Mouse_G2</t>
-  </si>
-  <si>
-    <t>Mouse_G3</t>
-  </si>
-  <si>
-    <t>Mouse_G4</t>
-  </si>
-  <si>
-    <t>Mouse_G5</t>
-  </si>
-  <si>
-    <t>Mouse_G6</t>
-  </si>
-  <si>
-    <t>Mouse_G7</t>
-  </si>
-  <si>
-    <t>Mouse_G8</t>
-  </si>
-  <si>
-    <t>Mouse_G9</t>
-  </si>
-  <si>
-    <t>Mouse_G10</t>
-  </si>
-  <si>
-    <t>Mouse_G11</t>
-  </si>
-  <si>
-    <t>Mouse_G12</t>
-  </si>
-  <si>
-    <t>RRP</t>
-  </si>
-  <si>
-    <t>Mouse_G13</t>
-  </si>
-  <si>
-    <t>LLP</t>
-  </si>
-  <si>
-    <t>Mouse_G14</t>
-  </si>
-  <si>
-    <t>RRLP</t>
-  </si>
-  <si>
-    <t>Mouse_G15</t>
-  </si>
-  <si>
-    <t>Mouse_G16</t>
-  </si>
-  <si>
-    <t>Mouse_G17</t>
-  </si>
-  <si>
-    <t>Mouse_G18</t>
-  </si>
-  <si>
-    <t>Mouse_G19</t>
-  </si>
-  <si>
-    <t>Mouse_G20</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,8 +594,7 @@
     <col min="5" max="5" width="36.6640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" style="1"/>
-    <col min="8" max="8" width="10.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -621,21 +620,21 @@
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E2" s="2">
         <v>44075</v>
@@ -644,24 +643,24 @@
         <v>888348</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2">
         <v>12</v>
-      </c>
-      <c r="H2" s="1">
-        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E3" s="2">
         <v>44075</v>
@@ -670,24 +669,24 @@
         <v>888048</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="1">
-        <v>261</v>
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2">
         <v>44235</v>
@@ -696,24 +695,24 @@
         <v>884393</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="1">
-        <v>101</v>
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2">
         <v>44235</v>
@@ -722,24 +721,24 @@
         <v>884393</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="1">
-        <v>101</v>
+        <v>11</v>
+      </c>
+      <c r="H5">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2">
         <v>44235</v>
@@ -748,24 +747,24 @@
         <v>884394</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="1">
-        <v>101</v>
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2">
         <v>44235</v>
@@ -774,24 +773,24 @@
         <v>884394</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="1">
-        <v>101</v>
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="2">
         <v>44249</v>
@@ -800,24 +799,24 @@
         <v>888048</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="1">
-        <v>87</v>
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="2">
         <v>44249</v>
@@ -826,24 +825,24 @@
         <v>888348</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="1">
-        <v>87</v>
+        <v>11</v>
+      </c>
+      <c r="H9">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>10</v>
-      </c>
       <c r="D10" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="7">
         <v>44317</v>
@@ -852,24 +851,24 @@
         <v>884394</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10">
         <v>12</v>
-      </c>
-      <c r="H10" s="1">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" s="7">
         <v>44317</v>
@@ -878,24 +877,24 @@
         <v>884394</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="1">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="H11">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="7">
         <v>44317</v>
@@ -904,24 +903,24 @@
         <v>884394</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="1">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="H12">
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" s="7">
         <v>44317</v>
@@ -930,24 +929,24 @@
         <v>884394</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="1">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="H13">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="7">
         <v>44317</v>
@@ -956,24 +955,24 @@
         <v>884395</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14">
         <v>12</v>
-      </c>
-      <c r="H14" s="1">
-        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="E15" s="7">
         <v>44317</v>
@@ -982,24 +981,24 @@
         <v>884395</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="1">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="H15">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16" s="7">
         <v>44317</v>
@@ -1008,24 +1007,24 @@
         <v>884395</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="1">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="H16">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" s="7">
         <v>44317</v>
@@ -1034,24 +1033,24 @@
         <v>884395</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17">
         <v>12</v>
-      </c>
-      <c r="H17" s="1">
-        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="E18" s="7">
         <v>44317</v>
@@ -1060,24 +1059,24 @@
         <v>884395</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="1">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="H18">
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E19" s="7">
         <v>44317</v>
@@ -1086,24 +1085,24 @@
         <v>884395</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="1">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="H19">
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E20" s="7">
         <v>44317</v>
@@ -1112,24 +1111,24 @@
         <v>884395</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" s="1">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="H20">
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>37</v>
-      </c>
       <c r="C21" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E21" s="7">
         <v>44317</v>
@@ -1138,24 +1137,24 @@
         <v>884395</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21">
         <v>12</v>
-      </c>
-      <c r="H21" s="1">
-        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>39</v>
-      </c>
       <c r="C22" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22" s="7">
         <v>44317</v>
@@ -1164,24 +1163,24 @@
         <v>884395</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="1">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="H22">
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="C23" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23" s="7">
         <v>44317</v>
@@ -1190,24 +1189,24 @@
         <v>884395</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" s="1">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="H23">
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" s="7">
         <v>44317</v>
@@ -1216,24 +1215,24 @@
         <v>884393</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H24" s="1">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="H24">
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="D25" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="E25" s="7">
         <v>44317</v>
@@ -1242,24 +1241,24 @@
         <v>884393</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25">
         <v>12</v>
-      </c>
-      <c r="H25" s="1">
-        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E26" s="7">
         <v>44317</v>
@@ -1268,24 +1267,24 @@
         <v>884393</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H26" s="1">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="H26">
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E27" s="7">
         <v>44317</v>
@@ -1294,24 +1293,24 @@
         <v>884393</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" s="1">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="H27">
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E28" s="7">
         <v>44317</v>
@@ -1320,24 +1319,24 @@
         <v>884393</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" s="1">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="H28">
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E29" s="7">
         <v>44317</v>
@@ -1346,10 +1345,10 @@
         <v>884393</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" s="1">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="H29">
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>